<commit_message>
Added documentation worked on during summer
</commit_message>
<xml_diff>
--- a/03 - Electrical Documentation/Wiring_Standard_BoM.xlsx
+++ b/03 - Electrical Documentation/Wiring_Standard_BoM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\1GitRepositories\GTOR\GTORDocumentation\03 - Electrical Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76451422-8195-45F9-8B72-BC876FA250CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E66532-8670-4624-A3BB-48F8BFF4993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4073" yWindow="893" windowWidth="15390" windowHeight="9532" xr2:uid="{7A4110FB-F398-44E2-99D0-D3932D447A86}"/>
+    <workbookView xWindow="4057" yWindow="3427" windowWidth="15390" windowHeight="9533" xr2:uid="{7A4110FB-F398-44E2-99D0-D3932D447A86}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Unit Price</t>
   </si>
@@ -90,24 +90,6 @@
     <t>Molex Micro-Fit</t>
   </si>
   <si>
-    <t>3 pin Molex Micro-Fit receptacle connector</t>
-  </si>
-  <si>
-    <t>3 pin Molex Micro-Fit plug connector</t>
-  </si>
-  <si>
-    <t>4 pin Molex Micro-Fit receptacle connector</t>
-  </si>
-  <si>
-    <t>4 pin Molex Micro-Fit plug connector</t>
-  </si>
-  <si>
-    <t>6 pin Molex Micro-Fit receptacle connector</t>
-  </si>
-  <si>
-    <t>6 pin Molex Micro-Fit plug connector</t>
-  </si>
-  <si>
     <t>Molex Micro-Fit female crimp</t>
   </si>
   <si>
@@ -117,21 +99,12 @@
     <t>https://www.digikey.com/en/products/detail/molex/0430450600/252528?s=N4IgTCBcDaICwGYAMcCsSBsSkgLoF8g</t>
   </si>
   <si>
-    <t>6 pin right angle Molex microfit receptacle connector</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/molex/0430450401/2405197?s=N4IgTCBcDaICwGYAMcCsKkEYQF0C%2BQA</t>
   </si>
   <si>
-    <t>4 pin right angle Molex microfit receptacle connector</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/molex/0436500300/268990?s=N4IgTCBcDaICwGYBsBWADGhGQF0C%2BQA</t>
   </si>
   <si>
-    <t>3 pin right angle Molex microfit receptacle connector</t>
-  </si>
-  <si>
     <t>Weather-Pack</t>
   </si>
   <si>
@@ -274,6 +247,42 @@
   </si>
   <si>
     <t>0.635mm CMC Recepticle plug</t>
+  </si>
+  <si>
+    <t>3-pin Molex Micro-Fit receptacle connector</t>
+  </si>
+  <si>
+    <t>3-pin Molex Micro-Fit plug connector</t>
+  </si>
+  <si>
+    <t>4-pin Molex Micro-Fit receptacle connector</t>
+  </si>
+  <si>
+    <t>4-pin Molex Micro-Fit plug connector</t>
+  </si>
+  <si>
+    <t>6-pin Molex Micro-Fit receptacle connector</t>
+  </si>
+  <si>
+    <t>6-pin Molex Micro-Fit plug connector</t>
+  </si>
+  <si>
+    <t>3-pin PCB-mount right angle Molex microfit receptacle connector</t>
+  </si>
+  <si>
+    <t>4-pin PCB-mount right angle Molex microfit receptacle connector</t>
+  </si>
+  <si>
+    <t>6-pin PCB-mount right angle Molex microfit receptacle connector</t>
+  </si>
+  <si>
+    <t>22 AWG 4-Core Signal Cable Unshielded</t>
+  </si>
+  <si>
+    <t>Silicone wire red</t>
+  </si>
+  <si>
+    <t>Silicone wire black</t>
   </si>
 </sst>
 </file>
@@ -843,8 +852,8 @@
   <dimension ref="A1:XFC39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -889,7 +898,7 @@
     </row>
     <row r="2" spans="1:8" s="16" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
@@ -901,30 +910,48 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D6" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -960,7 +987,7 @@
         <v>436450300</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -975,7 +1002,7 @@
         <v>436400301</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -990,7 +1017,7 @@
         <v>430250400</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1005,7 +1032,7 @@
         <v>430200401</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1020,7 +1047,7 @@
         <v>430250600</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1035,7 +1062,7 @@
         <v>430200601</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1044,13 +1071,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C18" s="10">
         <v>436500300</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1059,13 +1086,13 @@
         <v>8</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19" s="10">
         <v>430450401</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1074,13 +1101,13 @@
         <v>8</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" s="10">
         <v>430450600</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -1095,7 +1122,7 @@
         <v>430300051</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1110,7 +1137,7 @@
         <v>430315003</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1119,7 +1146,7 @@
     </row>
     <row r="24" spans="1:8" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="17" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -1131,63 +1158,63 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10">
         <v>12015792</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C26" s="10">
         <v>12010973</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="23" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -1202,13 +1229,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
@@ -1216,13 +1243,13 @@
         <v>8</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1230,13 +1257,13 @@
         <v>8</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1244,13 +1271,13 @@
         <v>8</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1258,13 +1285,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1272,13 +1299,13 @@
         <v>8</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1286,13 +1313,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1300,13 +1327,13 @@
         <v>8</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
@@ -1314,13 +1341,13 @@
         <v>8</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>